<commit_message>
Atualização de docstrings e arquivos de configuração
</commit_message>
<xml_diff>
--- a/ProjetoFinalCompass/Emails/E-mails para Notificações - RPA.xlsx
+++ b/ProjetoFinalCompass/Emails/E-mails para Notificações - RPA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ycaro\OneDrive\Área de Trabalho\RPA - Copia\ProjetoFinalCompass\Emails\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPA\ProjetoFinalCompass\Emails\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947DB1B3-14FD-4ECB-A450-EBD1D5AB93AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FA25B8-6584-45A9-9299-BCC8EDF987DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>ycarobanes@gmail.com</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -364,7 +368,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -373,7 +377,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -391,6 +397,9 @@
       <c r="J12" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{F41DC510-0043-4137-84C8-09F82E599729}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajustes e implementação de send_email_error
</commit_message>
<xml_diff>
--- a/ProjetoFinalCompass/Emails/E-mails para Notificações - RPA.xlsx
+++ b/ProjetoFinalCompass/Emails/E-mails para Notificações - RPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPA\ProjetoFinalCompass\Emails\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FA25B8-6584-45A9-9299-BCC8EDF987DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA18BB7-9E18-41C7-862E-AAE82F794CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>ycarobanes@gmail.com</t>
+    <t>notificacaorpachallenge@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -368,7 +368,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,6 +392,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J12" s="2"/>

</xml_diff>